<commit_message>
delete cancel purchase, dashboard
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tata\JOKI\Joki Feri UPB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4735F58-63D0-4747-84C0-0F2C35E344CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0340BBD6-171B-49CE-B126-854E16829E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11070" xr2:uid="{86D56B00-7E0B-428C-B370-1453DF00E845}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{86D56B00-7E0B-428C-B370-1453DF00E845}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,10 @@
     <t>SPAREPARTS</t>
   </si>
   <si>
-    <t>UUU</t>
+    <t>LED Vario 160</t>
   </si>
   <si>
-    <t>PT Mikuni</t>
+    <t>PT Kytaco Japan</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D50E1E-B8C5-4298-BDA2-10B92B446D4B}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>